<commit_message>
methods defined, html updated
Html now is closer to what final stage should be, all functionality now have their own methods with buttons assigned to them individually.
</commit_message>
<xml_diff>
--- a/Maintanence/Maintanence/bin/Debug/Book1.xlsx
+++ b/Maintanence/Maintanence/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9229e2ea6ea244ae"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R5cfeeb412e9d4b0a"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R39a9e1e83bd04d5d"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R373e2f10517148a9"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a5fe0d58-0a49-4077-b58d-843c6f8de341}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{bcd64dab-02fb-4028-9a71-496d84e9891c}">
   <we:reference id="83741d5a-1752-4f58-96b7-dd6dc2799ad7" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>